<commit_message>
Changed unemployment rate source
</commit_message>
<xml_diff>
--- a/data/unemploymentRate.xlsx
+++ b/data/unemploymentRate.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmainza/Desktop/projects/county-index/county-index/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E593FE-5F65-5047-8530-3029C2E83EEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EF11BB-FCEE-CD46-ACB1-63DAAC8F6260}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35560" yWindow="-940" windowWidth="27640" windowHeight="16940" xr2:uid="{29196C26-0591-BC4F-B1A5-2DA333DC3731}"/>
+    <workbookView xWindow="-33960" yWindow="-820" windowWidth="27640" windowHeight="16940" xr2:uid="{29196C26-0591-BC4F-B1A5-2DA333DC3731}"/>
   </bookViews>
   <sheets>
     <sheet name="blsAnnualRate" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +33,2397 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{002D7A9E-4C4A-FE46-9F17-18DF556DB019}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{EDBDFF34-E2F2-0D46-9FBC-42A4E2082565}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{E15FB206-7261-214A-9B76-DA91D114D469}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{380B717D-D5C3-2348-8961-B507693D01D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{2E1BD140-1DB9-DA40-B059-E1EE4624ACB6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{95A8AE03-BFF2-D14E-B824-0BF539722C41}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{9CF52E48-97BE-6343-B452-FC01CA0A88CE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{5310D1B3-0F22-D64F-83D8-7CA847F2EAED}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{B94FBD0F-CD18-4648-A6C0-418BAC57A16B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{232C4A3B-07A1-DB44-8BBD-9E7348EE0596}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{6D515856-5E0A-9243-8AAF-3FE6112F2F8C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="0" shapeId="0" xr:uid="{874E40C6-EC1F-A243-BDAF-5C852C98672B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{D063F8F3-D20E-AD4C-93F3-DC5F8D410D7C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M15" authorId="0" shapeId="0" xr:uid="{51638BA6-D5C2-1A40-BA06-DE67CAFCDC90}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M16" authorId="0" shapeId="0" xr:uid="{AEB52F9E-A02A-7449-BD99-6D01F0132183}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M17" authorId="0" shapeId="0" xr:uid="{C588EC47-AF8E-F94F-80B7-F43B4D716338}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M18" authorId="0" shapeId="0" xr:uid="{D1AD99D5-5DE9-AA4B-9904-CE741783BD03}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{E61FE2E6-09F4-8544-8A90-E115803BF27B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M20" authorId="0" shapeId="0" xr:uid="{D45FBDAF-4701-8842-B153-498B9D5D6290}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="0" shapeId="0" xr:uid="{BDFB620A-F19A-D740-9D99-B958B90C80C7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{144F7600-204A-DA4A-9E4F-42CB63BA0C5B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{71814529-F91B-8140-B7E5-127B8B6B62C2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M24" authorId="0" shapeId="0" xr:uid="{BF289E46-71A3-294E-9462-43A28EC5BF51}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M25" authorId="0" shapeId="0" xr:uid="{CF0CE186-7B45-0B45-A9CB-C7639102A977}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M26" authorId="0" shapeId="0" xr:uid="{F5F4FD71-A8C1-D64B-B5E9-6A3A6B05C8A2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{EB4304FD-A7B6-3F48-A758-F4B72F9BCD39}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{20AA3103-D4F7-7840-A52F-6488593EC18C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M29" authorId="0" shapeId="0" xr:uid="{258599B5-A066-B54D-82BF-26CF90CEB0A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M30" authorId="0" shapeId="0" xr:uid="{357BDF5F-C346-E044-971D-74AE9E419812}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M31" authorId="0" shapeId="0" xr:uid="{91CF2D27-3CBF-5841-BD6E-427801C95954}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M32" authorId="0" shapeId="0" xr:uid="{F7B9052A-2E5E-0345-9A48-594FDA093C36}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{A26E751D-F801-4A4F-8BE3-3F8D0C279168}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M34" authorId="0" shapeId="0" xr:uid="{00C79BC2-0610-7949-A896-7858242A7A57}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M35" authorId="0" shapeId="0" xr:uid="{5F43E8B4-CF01-4044-8A78-DDCF0BE7A93C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M36" authorId="0" shapeId="0" xr:uid="{16914AC0-96E9-2649-8FF3-49DFF6957E7B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M37" authorId="0" shapeId="0" xr:uid="{B60DE581-E451-5148-A3BE-C29E0F447C74}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M38" authorId="0" shapeId="0" xr:uid="{A4D6EC94-0D62-8D48-97F0-A223D6D471F8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M39" authorId="0" shapeId="0" xr:uid="{4CD2CF90-A911-E746-AA81-07C65FA11924}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M40" authorId="0" shapeId="0" xr:uid="{FF095A3E-FF3B-374F-93A3-4E8091E2E665}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M41" authorId="0" shapeId="0" xr:uid="{42F0FF46-0DCE-CC44-834A-1C589D36C94F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M42" authorId="0" shapeId="0" xr:uid="{0CAD69F8-878D-6649-B34E-0711F5BB2A32}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M43" authorId="0" shapeId="0" xr:uid="{3CE647B3-79CF-644D-A948-B6A3E34E2006}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M44" authorId="0" shapeId="0" xr:uid="{4ACD2FA3-AC47-9945-81F3-EF88751305DF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M45" authorId="0" shapeId="0" xr:uid="{F05F70D5-3652-AB46-9FD4-7C0902AED405}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M46" authorId="0" shapeId="0" xr:uid="{985EFE14-DE5B-414B-B816-CBA5BF98175A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M47" authorId="0" shapeId="0" xr:uid="{EC036066-24C6-114E-A105-4F0C39A78912}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M48" authorId="0" shapeId="0" xr:uid="{7E573CDF-57C0-144D-8F5A-DA5095BB700F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M49" authorId="0" shapeId="0" xr:uid="{FE953D25-62D1-304C-A896-DF6AACE81ADA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M50" authorId="0" shapeId="0" xr:uid="{57846445-041D-2841-AA11-4FDF3715F8CD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M51" authorId="0" shapeId="0" xr:uid="{4F0D4701-8516-C841-823E-2E3ABCD7D970}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M52" authorId="0" shapeId="0" xr:uid="{F84294F3-46BE-AA4E-932D-A867A4B24DB6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M53" authorId="0" shapeId="0" xr:uid="{65E6DA5D-C18E-BB48-8CF6-7B9A2AE13E15}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M54" authorId="0" shapeId="0" xr:uid="{40B51252-6BAB-2742-9DBD-F95F3F4F25FF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M55" authorId="0" shapeId="0" xr:uid="{7BCAF1F9-DA27-804B-AC29-6E95F6C785C7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M56" authorId="0" shapeId="0" xr:uid="{B4365900-A441-0C44-99EC-B47BA9276D6D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M57" authorId="0" shapeId="0" xr:uid="{9FF9CA46-A215-3B4A-BAC6-F882441613E4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M58" authorId="0" shapeId="0" xr:uid="{528B49C8-763C-8347-8ED5-99D4A5006A64}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M59" authorId="0" shapeId="0" xr:uid="{262BC9BE-3281-614A-9716-C3D1A75B590E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M60" authorId="0" shapeId="0" xr:uid="{54FC7EA7-63D6-2B4E-94BB-D9A7E6D86BC5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M61" authorId="0" shapeId="0" xr:uid="{D7B87367-4E93-5E4E-B778-1111D0768A1C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M62" authorId="0" shapeId="0" xr:uid="{2412E530-7F8C-AB40-847D-A1636F4965C8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M63" authorId="0" shapeId="0" xr:uid="{9A474F7E-3C22-9443-BC2A-00160F559A48}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M64" authorId="0" shapeId="0" xr:uid="{CB72067C-BE12-4A4D-882C-4314D88A475F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M65" authorId="0" shapeId="0" xr:uid="{2D702EFE-7226-9F4C-99FC-7D5B63A8BE54}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M66" authorId="0" shapeId="0" xr:uid="{3353ED29-AF88-FB43-8ED3-687AA99AD09B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M67" authorId="0" shapeId="0" xr:uid="{477C1637-5693-9341-B3DD-4F6FA51A8C8B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M68" authorId="0" shapeId="0" xr:uid="{F500D3A3-13FF-8147-AEED-B1525BDF4FB0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M69" authorId="0" shapeId="0" xr:uid="{977A5875-4A55-C749-9BC9-858B7D0B4D1A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M70" authorId="0" shapeId="0" xr:uid="{49CE40FA-8F9E-CE4F-A3C2-DF213212F640}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M71" authorId="0" shapeId="0" xr:uid="{EC8B23E0-028B-E045-82EB-732E47E68E1E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M72" authorId="0" shapeId="0" xr:uid="{9ED61A4E-FED8-0A43-9726-EA085EAF1692}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M73" authorId="0" shapeId="0" xr:uid="{1D326A0C-DBA9-5745-BF40-0D86969DF1DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M74" authorId="0" shapeId="0" xr:uid="{58E72BF4-F555-BF4F-97A4-E442309018D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M75" authorId="0" shapeId="0" xr:uid="{AA187A55-AC26-7148-A0DD-D1EDA7872532}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M76" authorId="0" shapeId="0" xr:uid="{82E2A823-7B28-F94C-B443-B54E248DA8F8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M77" authorId="0" shapeId="0" xr:uid="{ABE4C9EF-5614-8D44-A325-238397792E01}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M78" authorId="0" shapeId="0" xr:uid="{9F7E7C49-5860-904F-A449-330891C7D87B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M79" authorId="0" shapeId="0" xr:uid="{5CFACFEA-EBD6-4340-A14D-97E5FD8BC7A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M80" authorId="0" shapeId="0" xr:uid="{D1434C00-E754-1A48-9975-24C7CA6D90A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M81" authorId="0" shapeId="0" xr:uid="{FE20C05D-877D-074F-9959-1831DF81F5F4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M82" authorId="0" shapeId="0" xr:uid="{23439B33-ADFA-ED47-80F3-098F474D5E47}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M83" authorId="0" shapeId="0" xr:uid="{C63DB3E5-18D2-834C-A6ED-1182CE6DEC2E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M84" authorId="0" shapeId="0" xr:uid="{AAC9C4F9-ABCD-AF4B-ADFF-2F8D9884FA04}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M85" authorId="0" shapeId="0" xr:uid="{6CB6117E-5A39-4546-AB97-0583399D278A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M86" authorId="0" shapeId="0" xr:uid="{E1AA3221-AC8D-614F-8135-805CD0DAAF35}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M87" authorId="0" shapeId="0" xr:uid="{5BB46CA7-9991-2046-866E-AB6DBB1F33C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M88" authorId="0" shapeId="0" xr:uid="{7B45BFA7-1DEC-B549-9B29-B55A7598CFA5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M89" authorId="0" shapeId="0" xr:uid="{763493B4-3C63-F24C-8055-3F6C93BF0747}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M90" authorId="0" shapeId="0" xr:uid="{A4BA1C0E-0942-8948-B080-698E5FFA7AB7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M91" authorId="0" shapeId="0" xr:uid="{5A2A43D3-6918-8949-A562-AC7048AA2F9D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M92" authorId="0" shapeId="0" xr:uid="{F6AC442B-0A92-5D43-9E4B-D5BA45BD2CA1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M93" authorId="0" shapeId="0" xr:uid="{23BB574F-42E2-5C40-A402-02BF74A71FDF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M94" authorId="0" shapeId="0" xr:uid="{235D7A12-94D9-0B4A-A8C1-209F306E4597}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M95" authorId="0" shapeId="0" xr:uid="{7B3B3AFF-ADCB-4149-A536-65F4151ADD6F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M96" authorId="0" shapeId="0" xr:uid="{B8683CA5-8E6F-BF49-A907-83526D996E19}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M97" authorId="0" shapeId="0" xr:uid="{C9595AAE-4AC2-1F44-978D-B4E848B95F95}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M98" authorId="0" shapeId="0" xr:uid="{FB6CF2E4-3C76-FD46-B8CE-C463F127B343}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M99" authorId="0" shapeId="0" xr:uid="{DBDFF6DC-798A-724B-B976-94E8A12BCE5D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M100" authorId="0" shapeId="0" xr:uid="{297EBBBE-AF1C-ED4B-88C3-F11502CC2691}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M101" authorId="0" shapeId="0" xr:uid="{27019A95-66BD-724F-BBFC-E97656F9F0EE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M102" authorId="0" shapeId="0" xr:uid="{CD366723-6D72-E14A-832E-1C0A3146D673}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M103" authorId="0" shapeId="0" xr:uid="{05F1475D-A48F-AA43-B2A4-C08ACADCCC62}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M104" authorId="0" shapeId="0" xr:uid="{DB0E18AA-AD5A-7142-A11F-781B2A804EB8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M105" authorId="0" shapeId="0" xr:uid="{AD628A7D-CE08-044D-A0E3-E88F2637B396}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M106" authorId="0" shapeId="0" xr:uid="{AFEA9E45-9EDF-DC48-B209-40DB573DE454}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M107" authorId="0" shapeId="0" xr:uid="{EF4CB7A2-FA1C-4148-B548-BAFBB69FA902}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M108" authorId="0" shapeId="0" xr:uid="{0291F6FE-5F51-4B46-8BBF-FA5D4C9B5C40}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M109" authorId="0" shapeId="0" xr:uid="{D5082F43-B390-434F-A2B6-9EDFBE18945A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M110" authorId="0" shapeId="0" xr:uid="{0E6D33D8-EBB9-CE4E-8683-878F23350D32}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M111" authorId="0" shapeId="0" xr:uid="{720D882B-1E16-664F-9D58-1B2DDAEE9E46}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M112" authorId="0" shapeId="0" xr:uid="{A5860776-CFFD-9C42-AC07-E972F37AA676}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M113" authorId="0" shapeId="0" xr:uid="{AAB76F91-03EB-BA4A-AA57-E272C54AD581}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M114" authorId="0" shapeId="0" xr:uid="{2D117A5E-F2C8-DA40-B25F-42B9704297C0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M115" authorId="0" shapeId="0" xr:uid="{A2DF38DF-8BD4-EF40-9A9F-F58441FAE0A8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M116" authorId="0" shapeId="0" xr:uid="{0269D544-9F46-5B42-8DED-D8D7B09AEE66}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M117" authorId="0" shapeId="0" xr:uid="{78032B45-5CBF-9244-8008-9792E49D25C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M118" authorId="0" shapeId="0" xr:uid="{2B4BF8E0-D745-C349-9ED2-45581729B44D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M119" authorId="0" shapeId="0" xr:uid="{4EF59D0D-3545-824B-A635-70F1C3D5B4BF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M120" authorId="0" shapeId="0" xr:uid="{8C91E310-B256-A04B-81C2-664F8BF79F84}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M121" authorId="0" shapeId="0" xr:uid="{4BDADD03-9975-444B-95E8-114F9D70A5AC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M122" authorId="0" shapeId="0" xr:uid="{42C33007-AE22-1D41-98EE-172C4B5CCAD9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M123" authorId="0" shapeId="0" xr:uid="{829503B8-20C5-884C-BC92-0CFE534D8934}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M124" authorId="0" shapeId="0" xr:uid="{25D87DE3-9791-744C-A83F-66A6F72CE8A1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M125" authorId="0" shapeId="0" xr:uid="{F82AC676-C6B1-9046-A374-2259F457FB39}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M126" authorId="0" shapeId="0" xr:uid="{ECDE5CD6-BDD3-FE4B-A7D0-699822FFA446}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M127" authorId="0" shapeId="0" xr:uid="{19B70535-3408-4949-918A-656FAB23B780}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M128" authorId="0" shapeId="0" xr:uid="{5A8A1C7A-7CF2-3E48-A401-09B7B3548B90}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M129" authorId="0" shapeId="0" xr:uid="{55F1AF1B-1B52-FC4C-BBD1-C7005562760F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M130" authorId="0" shapeId="0" xr:uid="{691333B2-38DF-404C-BA38-FDAD40A1F3F0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M131" authorId="0" shapeId="0" xr:uid="{365E1AAA-EB7F-CC41-A112-37CA8566C025}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M132" authorId="0" shapeId="0" xr:uid="{62040CF8-B378-0C48-B338-EC8911FB0779}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M133" authorId="0" shapeId="0" xr:uid="{F03BDF19-7407-4F41-B240-418A98744E70}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M134" authorId="0" shapeId="0" xr:uid="{1BB088C0-4731-B74F-9516-CF4CD34505E1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M135" authorId="0" shapeId="0" xr:uid="{F880181C-0326-7D43-AE9B-6A0925D29F68}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M136" authorId="0" shapeId="0" xr:uid="{62770E80-97BE-C748-B013-3B4183F4394E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M137" authorId="0" shapeId="0" xr:uid="{B6A108A6-7F3A-4C47-A19D-5BE644A04638}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M138" authorId="0" shapeId="0" xr:uid="{0AAB0E91-9F74-0243-B25E-878DDAF6FBF6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M139" authorId="0" shapeId="0" xr:uid="{075DC3B9-B279-704C-A291-379C478B51EE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M140" authorId="0" shapeId="0" xr:uid="{62FB525F-6342-7348-A947-F734A0A051DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M141" authorId="0" shapeId="0" xr:uid="{E2CDEB56-DE26-D04E-B3B2-067C1A898D20}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M142" authorId="0" shapeId="0" xr:uid="{97366ADD-9EAE-9C43-84EC-582BD54D95E1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M143" authorId="0" shapeId="0" xr:uid="{796FA83E-14E0-E14F-918D-637AA1CD8235}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M144" authorId="0" shapeId="0" xr:uid="{A6C5E2B0-903E-D342-9325-BBC6CA2F57E1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M145" authorId="0" shapeId="0" xr:uid="{C7C42830-7A0A-BC4E-8F71-A4087C5A3DCF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M146" authorId="0" shapeId="0" xr:uid="{E0E3D6A5-EB38-1E40-869C-067BE0F6347F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M147" authorId="0" shapeId="0" xr:uid="{901522E2-DBD9-BF46-AF1D-BEEE7A0D01C9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M148" authorId="0" shapeId="0" xr:uid="{60058EA6-1880-B548-AB53-8DE593BBA72B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M149" authorId="0" shapeId="0" xr:uid="{7849476F-3004-D546-A5BC-C970E3037F65}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M150" authorId="0" shapeId="0" xr:uid="{1AF058A8-589C-2B41-ACF5-0A0D3ECD8E10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M151" authorId="0" shapeId="0" xr:uid="{A81D0540-F227-4D44-8787-5198E397E908}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M152" authorId="0" shapeId="0" xr:uid="{35EFDDB6-1A46-0244-A519-8BBC556F1490}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M153" authorId="0" shapeId="0" xr:uid="{D6D91535-6271-904D-BB06-EE5A3A56E145}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M154" authorId="0" shapeId="0" xr:uid="{CD7DB508-D421-B545-AD06-EF109D718F23}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M155" authorId="0" shapeId="0" xr:uid="{C04A5C1C-FD14-4945-98F5-BB3BD2C3EED4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M156" authorId="0" shapeId="0" xr:uid="{BF7079E9-12B4-BF47-B6F5-00D391A59697}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M157" authorId="0" shapeId="0" xr:uid="{EBCB8887-931A-5A49-B5A5-32870E84FA8A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M158" authorId="0" shapeId="0" xr:uid="{013022D0-D0E4-7C42-8F0F-336C93D743B9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M159" authorId="0" shapeId="0" xr:uid="{42EEBB90-FF2C-A743-8B86-E5A6E5C7378C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M160" authorId="0" shapeId="0" xr:uid="{CFA64705-3C0B-3C46-A02C-7684DCEF10D2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">*  Preliminary.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t>County</t>
   </si>
@@ -547,13 +2936,19 @@
   </si>
   <si>
     <t>2011 Unemployment Rate</t>
+  </si>
+  <si>
+    <t>2020 Unemployment Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,6 +2963,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -590,9 +3003,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,11 +3322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151A6857-B640-D443-8464-00907A694B40}">
-  <dimension ref="A1:L160"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151A6857-B640-D443-8464-00907A694B40}">
+  <dimension ref="A1:M160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,7 +3334,7 @@
     <col min="1" max="2" width="8.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -955,8 +3371,11 @@
       <c r="L1" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>13001</v>
       </c>
@@ -993,8 +3412,11 @@
       <c r="L2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13003</v>
       </c>
@@ -1031,8 +3453,11 @@
       <c r="L3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13005</v>
       </c>
@@ -1069,8 +3494,11 @@
       <c r="L4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13007</v>
       </c>
@@ -1107,8 +3535,11 @@
       <c r="L5">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>13009</v>
       </c>
@@ -1145,8 +3576,11 @@
       <c r="L6">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13011</v>
       </c>
@@ -1183,8 +3617,11 @@
       <c r="L7">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>13013</v>
       </c>
@@ -1221,8 +3658,11 @@
       <c r="L8">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>13015</v>
       </c>
@@ -1259,8 +3699,11 @@
       <c r="L9">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>13017</v>
       </c>
@@ -1297,8 +3740,11 @@
       <c r="L10">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="2">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>13019</v>
       </c>
@@ -1335,8 +3781,11 @@
       <c r="L11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13021</v>
       </c>
@@ -1373,8 +3822,11 @@
       <c r="L12">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="2">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13023</v>
       </c>
@@ -1411,8 +3863,11 @@
       <c r="L13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="2">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13025</v>
       </c>
@@ -1449,8 +3904,11 @@
       <c r="L14">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="2">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13027</v>
       </c>
@@ -1487,8 +3945,11 @@
       <c r="L15">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13029</v>
       </c>
@@ -1525,8 +3986,11 @@
       <c r="L16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13031</v>
       </c>
@@ -1563,8 +4027,11 @@
       <c r="L17">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="2">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>13033</v>
       </c>
@@ -1601,8 +4068,11 @@
       <c r="L18">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13035</v>
       </c>
@@ -1639,8 +4109,11 @@
       <c r="L19">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="2">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>13037</v>
       </c>
@@ -1677,8 +4150,11 @@
       <c r="L20">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>13039</v>
       </c>
@@ -1715,8 +4191,11 @@
       <c r="L21">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13043</v>
       </c>
@@ -1753,8 +4232,11 @@
       <c r="L22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>13045</v>
       </c>
@@ -1791,8 +4273,11 @@
       <c r="L23">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>13047</v>
       </c>
@@ -1829,8 +4314,11 @@
       <c r="L24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>13049</v>
       </c>
@@ -1867,8 +4355,11 @@
       <c r="L25">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13051</v>
       </c>
@@ -1905,8 +4396,11 @@
       <c r="L26">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="2">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13053</v>
       </c>
@@ -1943,8 +4437,11 @@
       <c r="L27">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="2">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>13055</v>
       </c>
@@ -1981,8 +4478,11 @@
       <c r="L28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" s="2">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>13057</v>
       </c>
@@ -2019,8 +4519,11 @@
       <c r="L29">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>13059</v>
       </c>
@@ -2057,8 +4560,11 @@
       <c r="L30">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" s="2">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13061</v>
       </c>
@@ -2095,8 +4601,11 @@
       <c r="L31">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" s="2">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>13063</v>
       </c>
@@ -2133,8 +4642,11 @@
       <c r="L32">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" s="2">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>13065</v>
       </c>
@@ -2171,8 +4683,11 @@
       <c r="L33">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>13067</v>
       </c>
@@ -2209,8 +4724,11 @@
       <c r="L34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>13069</v>
       </c>
@@ -2247,8 +4765,11 @@
       <c r="L35">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>13071</v>
       </c>
@@ -2285,8 +4806,11 @@
       <c r="L36">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>13073</v>
       </c>
@@ -2323,8 +4847,11 @@
       <c r="L37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>13075</v>
       </c>
@@ -2361,8 +4888,11 @@
       <c r="L38">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>13077</v>
       </c>
@@ -2399,8 +4929,11 @@
       <c r="L39">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>13079</v>
       </c>
@@ -2437,8 +4970,11 @@
       <c r="L40">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>13081</v>
       </c>
@@ -2475,8 +5011,11 @@
       <c r="L41">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" s="2">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>13083</v>
       </c>
@@ -2513,8 +5052,11 @@
       <c r="L42">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>13085</v>
       </c>
@@ -2551,8 +5093,11 @@
       <c r="L43">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>13087</v>
       </c>
@@ -2589,8 +5134,11 @@
       <c r="L44">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>13089</v>
       </c>
@@ -2627,8 +5175,11 @@
       <c r="L45">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" s="2">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>13091</v>
       </c>
@@ -2665,8 +5216,11 @@
       <c r="L46">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>13093</v>
       </c>
@@ -2703,8 +5257,11 @@
       <c r="L47">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>13095</v>
       </c>
@@ -2741,8 +5298,11 @@
       <c r="L48">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" s="2">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>13097</v>
       </c>
@@ -2779,8 +5339,11 @@
       <c r="L49">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>13099</v>
       </c>
@@ -2817,8 +5380,11 @@
       <c r="L50">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>13101</v>
       </c>
@@ -2855,8 +5421,11 @@
       <c r="L51">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>13103</v>
       </c>
@@ -2893,8 +5462,11 @@
       <c r="L52">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>13105</v>
       </c>
@@ -2931,8 +5503,11 @@
       <c r="L53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>13107</v>
       </c>
@@ -2969,8 +5544,11 @@
       <c r="L54">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" s="2">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>13109</v>
       </c>
@@ -3007,8 +5585,11 @@
       <c r="L55">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>13111</v>
       </c>
@@ -3045,8 +5626,11 @@
       <c r="L56">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" s="2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>13113</v>
       </c>
@@ -3083,8 +5667,11 @@
       <c r="L57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>13115</v>
       </c>
@@ -3121,8 +5708,11 @@
       <c r="L58">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>13117</v>
       </c>
@@ -3159,8 +5749,11 @@
       <c r="L59">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>13119</v>
       </c>
@@ -3197,8 +5790,11 @@
       <c r="L60">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>13121</v>
       </c>
@@ -3235,8 +5831,11 @@
       <c r="L61">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>13123</v>
       </c>
@@ -3273,8 +5872,11 @@
       <c r="L62">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>13125</v>
       </c>
@@ -3311,8 +5913,11 @@
       <c r="L63">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>13127</v>
       </c>
@@ -3349,8 +5954,11 @@
       <c r="L64">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>13129</v>
       </c>
@@ -3387,8 +5995,11 @@
       <c r="L65">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" s="2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>13131</v>
       </c>
@@ -3425,8 +6036,11 @@
       <c r="L66">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>13133</v>
       </c>
@@ -3463,8 +6077,11 @@
       <c r="L67">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>13135</v>
       </c>
@@ -3501,8 +6118,11 @@
       <c r="L68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>13137</v>
       </c>
@@ -3539,8 +6159,11 @@
       <c r="L69">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>13139</v>
       </c>
@@ -3577,8 +6200,11 @@
       <c r="L70">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" s="2">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>13141</v>
       </c>
@@ -3615,8 +6241,11 @@
       <c r="L71">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" s="2">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>13143</v>
       </c>
@@ -3653,8 +6282,11 @@
       <c r="L72">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M72" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>13145</v>
       </c>
@@ -3691,8 +6323,11 @@
       <c r="L73">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>13147</v>
       </c>
@@ -3729,8 +6364,11 @@
       <c r="L74">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>13149</v>
       </c>
@@ -3767,8 +6405,11 @@
       <c r="L75">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>13151</v>
       </c>
@@ -3805,8 +6446,11 @@
       <c r="L76">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>13153</v>
       </c>
@@ -3843,8 +6487,11 @@
       <c r="L77">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M77" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>13155</v>
       </c>
@@ -3881,8 +6528,11 @@
       <c r="L78">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M78" s="2">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>13157</v>
       </c>
@@ -3919,8 +6569,11 @@
       <c r="L79">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M79" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>13159</v>
       </c>
@@ -3957,8 +6610,11 @@
       <c r="L80">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M80" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>13161</v>
       </c>
@@ -3995,8 +6651,11 @@
       <c r="L81">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M81" s="2">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>13163</v>
       </c>
@@ -4033,8 +6692,11 @@
       <c r="L82">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M82" s="2">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>13165</v>
       </c>
@@ -4071,8 +6733,11 @@
       <c r="L83">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M83" s="2">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>13167</v>
       </c>
@@ -4109,8 +6774,11 @@
       <c r="L84">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M84" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>13169</v>
       </c>
@@ -4147,8 +6815,11 @@
       <c r="L85">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M85" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>13171</v>
       </c>
@@ -4185,8 +6856,11 @@
       <c r="L86">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M86" s="2">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>13173</v>
       </c>
@@ -4223,8 +6897,11 @@
       <c r="L87">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M87" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>13175</v>
       </c>
@@ -4261,8 +6938,11 @@
       <c r="L88">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M88" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>13177</v>
       </c>
@@ -4299,8 +6979,11 @@
       <c r="L89">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M89" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>13179</v>
       </c>
@@ -4337,8 +7020,11 @@
       <c r="L90">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M90" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>13181</v>
       </c>
@@ -4375,8 +7061,11 @@
       <c r="L91">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M91" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>13183</v>
       </c>
@@ -4413,8 +7102,11 @@
       <c r="L92">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M92" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>13185</v>
       </c>
@@ -4451,8 +7143,11 @@
       <c r="L93">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M93" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>13187</v>
       </c>
@@ -4489,8 +7184,11 @@
       <c r="L94">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M94" s="2">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>13189</v>
       </c>
@@ -4527,8 +7225,11 @@
       <c r="L95">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M95" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>13191</v>
       </c>
@@ -4565,8 +7266,11 @@
       <c r="L96">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M96" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>13193</v>
       </c>
@@ -4603,8 +7307,11 @@
       <c r="L97">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M97" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>13195</v>
       </c>
@@ -4641,8 +7348,11 @@
       <c r="L98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M98" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>13197</v>
       </c>
@@ -4679,8 +7389,11 @@
       <c r="L99">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M99" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>13199</v>
       </c>
@@ -4717,8 +7430,11 @@
       <c r="L100">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M100" s="2">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>13201</v>
       </c>
@@ -4755,8 +7471,11 @@
       <c r="L101">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M101" s="2">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>13205</v>
       </c>
@@ -4793,8 +7512,11 @@
       <c r="L102">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M102" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>13207</v>
       </c>
@@ -4831,8 +7553,11 @@
       <c r="L103">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M103" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>13209</v>
       </c>
@@ -4869,8 +7594,11 @@
       <c r="L104">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M104" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>13211</v>
       </c>
@@ -4907,8 +7635,11 @@
       <c r="L105">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M105" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>13213</v>
       </c>
@@ -4945,8 +7676,11 @@
       <c r="L106">
         <v>5</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M106" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>13215</v>
       </c>
@@ -4983,8 +7717,11 @@
       <c r="L107">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M107" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>13217</v>
       </c>
@@ -5021,8 +7758,11 @@
       <c r="L108">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M108" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>13219</v>
       </c>
@@ -5059,8 +7799,11 @@
       <c r="L109">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M109" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>13221</v>
       </c>
@@ -5097,8 +7840,11 @@
       <c r="L110">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M110" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>13223</v>
       </c>
@@ -5135,8 +7881,11 @@
       <c r="L111">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M111" s="2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>13225</v>
       </c>
@@ -5173,8 +7922,11 @@
       <c r="L112">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M112" s="2">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>13227</v>
       </c>
@@ -5211,8 +7963,11 @@
       <c r="L113">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M113" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>13229</v>
       </c>
@@ -5249,8 +8004,11 @@
       <c r="L114">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M114" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>13231</v>
       </c>
@@ -5287,8 +8045,11 @@
       <c r="L115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M115" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>13233</v>
       </c>
@@ -5325,8 +8086,11 @@
       <c r="L116">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M116" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>13235</v>
       </c>
@@ -5363,8 +8127,11 @@
       <c r="L117">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M117" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>13237</v>
       </c>
@@ -5401,8 +8168,11 @@
       <c r="L118">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M118" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>13239</v>
       </c>
@@ -5439,8 +8209,11 @@
       <c r="L119">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M119" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>13241</v>
       </c>
@@ -5477,8 +8250,11 @@
       <c r="L120">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M120" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>13243</v>
       </c>
@@ -5515,8 +8291,11 @@
       <c r="L121">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M121" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>13245</v>
       </c>
@@ -5553,8 +8332,11 @@
       <c r="L122">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M122" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>13247</v>
       </c>
@@ -5591,8 +8373,11 @@
       <c r="L123">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M123" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>13249</v>
       </c>
@@ -5629,8 +8414,11 @@
       <c r="L124">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M124" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>13251</v>
       </c>
@@ -5667,8 +8455,11 @@
       <c r="L125">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M125" s="2">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>13253</v>
       </c>
@@ -5705,8 +8496,11 @@
       <c r="L126">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M126" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>13255</v>
       </c>
@@ -5743,8 +8537,11 @@
       <c r="L127">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M127" s="2">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>13257</v>
       </c>
@@ -5781,8 +8578,11 @@
       <c r="L128">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M128" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>13259</v>
       </c>
@@ -5819,8 +8619,11 @@
       <c r="L129">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M129" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>13261</v>
       </c>
@@ -5857,8 +8660,11 @@
       <c r="L130">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M130" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>13263</v>
       </c>
@@ -5895,8 +8701,11 @@
       <c r="L131">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M131" s="2">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>13265</v>
       </c>
@@ -5933,8 +8742,11 @@
       <c r="L132">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M132" s="2">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>13267</v>
       </c>
@@ -5971,8 +8783,11 @@
       <c r="L133">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M133" s="2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>13269</v>
       </c>
@@ -6009,8 +8824,11 @@
       <c r="L134">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M134" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>13271</v>
       </c>
@@ -6047,8 +8865,11 @@
       <c r="L135">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M135" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>13273</v>
       </c>
@@ -6085,8 +8906,11 @@
       <c r="L136">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M136" s="2">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>13275</v>
       </c>
@@ -6123,8 +8947,11 @@
       <c r="L137">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M137" s="2">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>13277</v>
       </c>
@@ -6161,8 +8988,11 @@
       <c r="L138">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M138" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>13279</v>
       </c>
@@ -6199,8 +9029,11 @@
       <c r="L139">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M139" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>13281</v>
       </c>
@@ -6237,8 +9070,11 @@
       <c r="L140">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M140" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>13283</v>
       </c>
@@ -6275,8 +9111,11 @@
       <c r="L141">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M141" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>13285</v>
       </c>
@@ -6313,8 +9152,11 @@
       <c r="L142">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M142" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>13287</v>
       </c>
@@ -6351,8 +9193,11 @@
       <c r="L143">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M143" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>13289</v>
       </c>
@@ -6389,8 +9234,11 @@
       <c r="L144">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M144" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>13291</v>
       </c>
@@ -6427,8 +9275,11 @@
       <c r="L145">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M145" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>13293</v>
       </c>
@@ -6465,8 +9316,11 @@
       <c r="L146">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M146" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>13295</v>
       </c>
@@ -6503,8 +9357,11 @@
       <c r="L147">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M147" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>13297</v>
       </c>
@@ -6541,8 +9398,11 @@
       <c r="L148">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M148" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>13299</v>
       </c>
@@ -6579,8 +9439,11 @@
       <c r="L149">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M149" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>13301</v>
       </c>
@@ -6617,8 +9480,11 @@
       <c r="L150">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M150" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>13303</v>
       </c>
@@ -6655,8 +9521,11 @@
       <c r="L151">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M151" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>13305</v>
       </c>
@@ -6693,8 +9562,11 @@
       <c r="L152">
         <v>4</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M152" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>13307</v>
       </c>
@@ -6731,8 +9603,11 @@
       <c r="L153">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M153" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>13309</v>
       </c>
@@ -6769,8 +9644,11 @@
       <c r="L154">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M154" s="2">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>13311</v>
       </c>
@@ -6807,8 +9685,11 @@
       <c r="L155">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M155" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>13313</v>
       </c>
@@ -6845,8 +9726,11 @@
       <c r="L156">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M156" s="2">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>13315</v>
       </c>
@@ -6883,8 +9767,11 @@
       <c r="L157">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M157" s="2">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>13317</v>
       </c>
@@ -6921,8 +9808,11 @@
       <c r="L158">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M158" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>13319</v>
       </c>
@@ -6959,8 +9849,11 @@
       <c r="L159">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M159" s="2">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>13321</v>
       </c>
@@ -6997,8 +9890,12 @@
       <c r="L160">
         <v>3.9</v>
       </c>
+      <c r="M160" s="2">
+        <v>5.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>